<commit_message>
fixes levels of release metadata, writes and validates xml
</commit_message>
<xml_diff>
--- a/data-raw/metadata/tisdale_release_metadata.xlsx
+++ b/data-raw/metadata/tisdale_release_metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Badhia\Documents\git\jpe-tisdale-edi\data-raw\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{675FC19C-0A99-4BC0-884A-356148E4C99C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3131F84D-9736-4827-8043-F02D1D90CAFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4260" yWindow="2290" windowWidth="19200" windowHeight="11170" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5550" yWindow="1780" windowWidth="16860" windowHeight="13080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="attribute" sheetId="1" r:id="rId1"/>
@@ -186,9 +186,6 @@
     <t>Origin or production type of fish marked. Levels =c("Unknown", "Natural", "Not recorded", "Hatchery")</t>
   </si>
   <si>
-    <t>Site where fish were released. Levels = c("Knights Landing release site", "Not applicable")</t>
-  </si>
-  <si>
     <t>Mark type that was applied to the release group. Levels = c("Pigment / dye", "Fin clip", "Elastomer", NA)</t>
   </si>
   <si>
@@ -233,6 +230,9 @@
   </si>
   <si>
     <t>enumerated</t>
+  </si>
+  <si>
+    <t>Site where fish were released. Levels = c("Tisdale Weir release site")</t>
   </si>
 </sst>
 </file>
@@ -359,14 +359,14 @@
     <xf numFmtId="14" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -584,8 +584,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z993"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -664,7 +664,7 @@
         <v>13</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>18</v>
@@ -673,7 +673,7 @@
         <v>15</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
@@ -778,7 +778,7 @@
         <v>38</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>14</v>
@@ -816,7 +816,7 @@
         <v>39</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>14</v>
@@ -892,7 +892,7 @@
         <v>43</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>14</v>
@@ -930,7 +930,7 @@
         <v>44</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>49</v>
+        <v>64</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>14</v>
@@ -1074,10 +1074,10 @@
       </c>
       <c r="K12" s="2"/>
       <c r="L12" s="14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="M12" s="14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
@@ -1146,7 +1146,7 @@
         <v>41</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>14</v>
@@ -1184,7 +1184,7 @@
         <v>42</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>14</v>
@@ -1222,7 +1222,7 @@
         <v>46</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>14</v>
@@ -1257,10 +1257,10 @@
     </row>
     <row r="17" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>14</v>
@@ -1295,10 +1295,10 @@
     </row>
     <row r="18" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>14</v>
@@ -1640,7 +1640,7 @@
       <c r="Z29" s="1"/>
     </row>
     <row r="30" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="22"/>
+      <c r="A30" s="24"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
       <c r="D30" s="2"/>
@@ -1668,7 +1668,7 @@
       <c r="Z30" s="1"/>
     </row>
     <row r="31" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="23"/>
+      <c r="A31" s="25"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
       <c r="D31" s="2"/>
@@ -1696,7 +1696,7 @@
       <c r="Z31" s="1"/>
     </row>
     <row r="32" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="22"/>
+      <c r="A32" s="24"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
       <c r="D32" s="2"/>
@@ -1724,7 +1724,7 @@
       <c r="Z32" s="1"/>
     </row>
     <row r="33" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="23"/>
+      <c r="A33" s="25"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
       <c r="D33" s="2"/>
@@ -28659,7 +28659,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z666"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
@@ -28706,13 +28706,13 @@
       <c r="Z1" s="13"/>
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="24">
+      <c r="A2" s="22">
         <v>10</v>
       </c>
-      <c r="B2" s="25" t="s">
-        <v>63</v>
+      <c r="B2" s="23" t="s">
+        <v>62</v>
       </c>
-      <c r="C2" s="24" t="s">
+      <c r="C2" s="22" t="s">
         <v>13</v>
       </c>
       <c r="D2" s="13"/>

</xml_diff>